<commit_message>
** Push for fun **
</commit_message>
<xml_diff>
--- a/Magnetometer/NoiseFloor_raw_withGraph.xlsx
+++ b/Magnetometer/NoiseFloor_raw_withGraph.xlsx
@@ -571,37 +571,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -636,6 +606,36 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="8"/>
+              <c:pt idx="0">
+                <c:v>0</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>7</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>NoiseFloor_raw!$A$102:$H$102</c:f>
@@ -1737,7 +1737,7 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>